<commit_message>
TFG: Entity-Relationship Diagram (not completed)
</commit_message>
<xml_diff>
--- a/TFG/TFG Diagrama de Gantt.xlsx
+++ b/TFG/TFG Diagrama de Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58715E2F-DEC8-2B48-A525-3DCA97ABEC2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536AC0F-BA09-524A-B34A-FC3B63F1811D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -118,12 +118,6 @@
   </si>
   <si>
     <t>TAREA</t>
-  </si>
-  <si>
-    <t>Tarea 2</t>
-  </si>
-  <si>
-    <t>Tarea 3</t>
   </si>
   <si>
     <t>Tarea 4</t>
@@ -233,9 +227,6 @@
     <t>Elaboración de ítems a llevar a cabo</t>
   </si>
   <si>
-    <t>Formación en SwiftUI (Framework de Swift para aplicaciones iOS)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Elaboración logo </t>
     </r>
@@ -316,25 +307,22 @@
     <t>Conexión de la API privada con el front-end</t>
   </si>
   <si>
-    <t>Diagrama de casos de uso: Entrenador</t>
+    <t>Inserción de ejercicios</t>
   </si>
   <si>
-    <t>Estructura por capas del Entrenador</t>
+    <t>Diagrama de casos de uso</t>
   </si>
   <si>
-    <t>Estructura por capas del Deportista</t>
+    <t>Formación: Swift</t>
   </si>
   <si>
-    <t>Diagrama de casos de uso: Deportista</t>
+    <t>Formación: SwiftUI</t>
   </si>
   <si>
-    <t>CRUD básico del Entrenador</t>
+    <t>CRUD básico</t>
   </si>
   <si>
-    <t>CRUD básico del Deportista</t>
-  </si>
-  <si>
-    <t>Inserción de ejercicios</t>
+    <t>Estructura por capas</t>
   </si>
 </sst>
 </file>
@@ -1449,53 +1437,7 @@
     <cellStyle name="Warning Text" xfId="26" builtinId="11" customBuiltin="1"/>
     <cellStyle name="zTextoOculto" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -1645,15 +1587,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ListaTareasPendientes" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="17"/>
-      <tableStyleElement type="headerRow" dxfId="16"/>
-      <tableStyleElement type="totalRow" dxfId="15"/>
-      <tableStyleElement type="firstColumn" dxfId="14"/>
-      <tableStyleElement type="lastColumn" dxfId="13"/>
-      <tableStyleElement type="firstRowStripe" dxfId="12"/>
-      <tableStyleElement type="secondRowStripe" dxfId="11"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="10"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="lastColumn" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="secondRowStripe" dxfId="7"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="6"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="5"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2068,11 +2010,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BY42"/>
+  <dimension ref="A1:BY41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2093,14 +2035,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="29"/>
       <c r="G1" s="1"/>
       <c r="H1" s="52" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,7 +2051,7 @@
       </c>
       <c r="B2" s="44"/>
       <c r="H2" s="53" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2118,7 +2060,7 @@
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="76" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D3" s="80">
         <v>45719</v>
@@ -2532,17 +2474,17 @@
         <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H6" s="8" t="str">
         <f t="shared" ref="H6" si="13">LEFT(TEXT(H5,"ddd"),1)</f>
@@ -2910,14 +2852,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="55"/>
       <c r="E8" s="56"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="str">
-        <f t="shared" ref="G8:G40" si="18">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G8:G39" si="18">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H8" s="26"/>
@@ -2996,7 +2938,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -3089,7 +3031,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
@@ -3181,7 +3123,7 @@
     <row r="11" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="13">
         <v>1</v>
@@ -3272,7 +3214,7 @@
     <row r="12" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C12" s="13">
         <v>1</v>
@@ -3362,7 +3304,7 @@
     <row r="13" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="46" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C13" s="13">
         <v>0.2</v>
@@ -3371,8 +3313,7 @@
         <v>45722</v>
       </c>
       <c r="E13" s="57">
-        <f>D13+4</f>
-        <v>45726</v>
+        <v>45730</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
@@ -3450,11 +3391,15 @@
     <row r="14" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="46" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="13"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
+      <c r="D14" s="57">
+        <v>45732</v>
+      </c>
+      <c r="E14" s="57">
+        <v>45735</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="26"/>
@@ -3530,12 +3475,16 @@
     </row>
     <row r="15" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
-      <c r="B15" s="46" t="s">
-        <v>62</v>
+      <c r="B15" s="73" t="s">
+        <v>49</v>
       </c>
       <c r="C15" s="13"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
+      <c r="D15" s="57">
+        <v>45736</v>
+      </c>
+      <c r="E15" s="57">
+        <v>45736</v>
+      </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
       <c r="H15" s="26"/>
@@ -3611,9 +3560,7 @@
     </row>
     <row r="16" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="40"/>
-      <c r="B16" s="73" t="s">
-        <v>52</v>
-      </c>
+      <c r="B16" s="73"/>
       <c r="C16" s="13"/>
       <c r="D16" s="57"/>
       <c r="E16" s="57"/>
@@ -3693,7 +3640,7 @@
     <row r="17" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="46" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="57">
@@ -3785,7 +3732,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="58"/>
@@ -3869,22 +3816,21 @@
     <row r="19" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="47" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" s="16">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D19" s="60">
-        <v>45722</v>
+        <v>45735</v>
       </c>
       <c r="E19" s="60">
-        <f>D19+4</f>
-        <v>45726</v>
+        <v>45737</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10">
         <f t="shared" si="18"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
@@ -3960,22 +3906,21 @@
     <row r="20" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="47" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C20" s="16">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D20" s="60">
-        <v>45726</v>
+        <v>45738</v>
       </c>
       <c r="E20" s="60">
-        <f>D20+5</f>
-        <v>45731</v>
+        <v>45741</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10">
         <f t="shared" si="18"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
@@ -4051,20 +3996,19 @@
     <row r="21" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="47" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C21" s="16"/>
       <c r="D21" s="60">
-        <v>45727</v>
+        <v>45742</v>
       </c>
       <c r="E21" s="60">
-        <f>D21+3</f>
-        <v>45730</v>
+        <v>45746</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -4140,16 +4084,16 @@
     <row r="22" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="40"/>
       <c r="B22" s="47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C22" s="16"/>
       <c r="D22" s="60">
         <f>D21</f>
-        <v>45727</v>
+        <v>45742</v>
       </c>
       <c r="E22" s="60">
         <f>D22+2</f>
-        <v>45729</v>
+        <v>45744</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10">
@@ -4230,16 +4174,16 @@
     <row r="23" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
       <c r="B23" s="47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C23" s="16"/>
       <c r="D23" s="60">
         <f>D22</f>
-        <v>45727</v>
+        <v>45742</v>
       </c>
       <c r="E23" s="60">
         <f>D23+3</f>
-        <v>45730</v>
+        <v>45745</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10">
@@ -4322,7 +4266,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="18"/>
       <c r="D24" s="61"/>
@@ -4406,7 +4350,7 @@
     <row r="25" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="48" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C25" s="19"/>
       <c r="D25" s="63">
@@ -4496,14 +4440,14 @@
     <row r="26" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="48" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C26" s="19"/>
       <c r="D26" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E26" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10" t="e">
@@ -4584,14 +4528,14 @@
     <row r="27" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="19"/>
       <c r="D27" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E27" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10" t="e">
@@ -4671,15 +4615,13 @@
     </row>
     <row r="28" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
-      <c r="B28" s="48" t="s">
-        <v>63</v>
-      </c>
+      <c r="B28" s="48"/>
       <c r="C28" s="19"/>
       <c r="D28" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E28" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="e">
@@ -4759,9 +4701,7 @@
     </row>
     <row r="29" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
-      <c r="B29" s="48" t="s">
-        <v>64</v>
-      </c>
+      <c r="B29" s="48"/>
       <c r="C29" s="19"/>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
@@ -4920,14 +4860,14 @@
     <row r="31" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="48" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31" s="63" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="e">
@@ -5010,7 +4950,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="64"/>
@@ -5094,9 +5034,11 @@
     <row r="33" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="22"/>
+        <v>59</v>
+      </c>
+      <c r="C33" s="22">
+        <v>1</v>
+      </c>
       <c r="D33" s="66">
         <v>45727</v>
       </c>
@@ -5182,19 +5124,21 @@
     <row r="34" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="22"/>
-      <c r="D34" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="E34" s="66" t="s">
-        <v>22</v>
+        <v>58</v>
+      </c>
+      <c r="C34" s="22">
+        <v>1</v>
+      </c>
+      <c r="D34" s="66">
+        <v>45734</v>
+      </c>
+      <c r="E34" s="66">
+        <v>45741</v>
       </c>
       <c r="F34" s="10"/>
-      <c r="G34" s="10" t="e">
+      <c r="G34" s="10">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v>8</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -5270,14 +5214,14 @@
     <row r="35" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="49" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C35" s="22"/>
       <c r="D35" s="66" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E35" s="66" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F35" s="10"/>
       <c r="G35" s="10" t="e">
@@ -5358,20 +5302,17 @@
     <row r="36" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
       <c r="B36" s="49" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="C36" s="22"/>
-      <c r="D36" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="E36" s="66" t="s">
-        <v>22</v>
+      <c r="D36" s="66">
+        <v>45778</v>
+      </c>
+      <c r="E36" s="66">
+        <v>45779</v>
       </c>
       <c r="F36" s="10"/>
-      <c r="G36" s="10" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G36" s="10"/>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
       <c r="J36" s="26"/>
@@ -5446,17 +5387,20 @@
     <row r="37" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
       <c r="B37" s="49" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="C37" s="22"/>
-      <c r="D37" s="66">
-        <v>45778</v>
-      </c>
-      <c r="E37" s="66">
-        <v>45779</v>
+      <c r="D37" s="66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>20</v>
       </c>
       <c r="F37" s="10"/>
-      <c r="G37" s="10"/>
+      <c r="G37" s="10" t="e">
+        <f t="shared" si="18"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
       <c r="J37" s="26"/>
@@ -5529,21 +5473,24 @@
       <c r="BY37" s="26"/>
     </row>
     <row r="38" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="49" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="22"/>
-      <c r="D38" s="66" t="s">
-        <v>22</v>
-      </c>
-      <c r="E38" s="66" t="s">
-        <v>22</v>
+      <c r="A38" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="50" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="9"/>
+      <c r="D38" s="67">
+        <v>45782</v>
+      </c>
+      <c r="E38" s="67">
+        <f>D38+5</f>
+        <v>45787</v>
       </c>
       <c r="F38" s="10"/>
-      <c r="G38" s="10" t="e">
+      <c r="G38" s="10">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v>6</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -5617,187 +5564,96 @@
       <c r="BY38" s="26"/>
     </row>
     <row r="39" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="67">
-        <v>45782</v>
-      </c>
-      <c r="E39" s="67">
-        <f>D39+5</f>
-        <v>45787</v>
-      </c>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10">
-        <f t="shared" si="18"/>
-        <v>6</v>
-      </c>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="26"/>
-      <c r="K39" s="26"/>
-      <c r="L39" s="26"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="26"/>
-      <c r="Q39" s="26"/>
-      <c r="R39" s="26"/>
-      <c r="S39" s="26"/>
-      <c r="T39" s="26"/>
-      <c r="U39" s="26"/>
-      <c r="V39" s="26"/>
-      <c r="W39" s="26"/>
-      <c r="X39" s="26"/>
-      <c r="Y39" s="26"/>
-      <c r="Z39" s="26"/>
-      <c r="AA39" s="26"/>
-      <c r="AB39" s="26"/>
-      <c r="AC39" s="26"/>
-      <c r="AD39" s="26"/>
-      <c r="AE39" s="26"/>
-      <c r="AF39" s="26"/>
-      <c r="AG39" s="26"/>
-      <c r="AH39" s="26"/>
-      <c r="AI39" s="26"/>
-      <c r="AJ39" s="26"/>
-      <c r="AK39" s="26"/>
-      <c r="AL39" s="26"/>
-      <c r="AM39" s="26"/>
-      <c r="AN39" s="26"/>
-      <c r="AO39" s="26"/>
-      <c r="AP39" s="26"/>
-      <c r="AQ39" s="26"/>
-      <c r="AR39" s="26"/>
-      <c r="AS39" s="26"/>
-      <c r="AT39" s="26"/>
-      <c r="AU39" s="26"/>
-      <c r="AV39" s="26"/>
-      <c r="AW39" s="26"/>
-      <c r="AX39" s="26"/>
-      <c r="AY39" s="26"/>
-      <c r="AZ39" s="26"/>
-      <c r="BA39" s="26"/>
-      <c r="BB39" s="26"/>
-      <c r="BC39" s="26"/>
-      <c r="BD39" s="26"/>
-      <c r="BE39" s="26"/>
-      <c r="BF39" s="26"/>
-      <c r="BG39" s="26"/>
-      <c r="BH39" s="26"/>
-      <c r="BI39" s="26"/>
-      <c r="BJ39" s="26"/>
-      <c r="BK39" s="26"/>
-      <c r="BL39" s="26"/>
-      <c r="BM39" s="26"/>
-      <c r="BN39" s="26"/>
-      <c r="BO39" s="26"/>
-      <c r="BP39" s="26"/>
-      <c r="BQ39" s="26"/>
-      <c r="BR39" s="26"/>
-      <c r="BS39" s="26"/>
-      <c r="BT39" s="26"/>
-      <c r="BU39" s="26"/>
-      <c r="BV39" s="26"/>
-      <c r="BW39" s="26"/>
-      <c r="BX39" s="26"/>
-      <c r="BY39" s="26"/>
-    </row>
-    <row r="40" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="41" t="s">
+      <c r="A39" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B40" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="24"/>
-      <c r="D40" s="68"/>
-      <c r="E40" s="69"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25" t="str">
+      <c r="B39" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="24"/>
+      <c r="D39" s="68"/>
+      <c r="E39" s="69"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="H40" s="28"/>
-      <c r="I40" s="28"/>
-      <c r="J40" s="28"/>
-      <c r="K40" s="28"/>
-      <c r="L40" s="28"/>
-      <c r="M40" s="28"/>
-      <c r="N40" s="28"/>
-      <c r="O40" s="28"/>
-      <c r="P40" s="28"/>
-      <c r="Q40" s="28"/>
-      <c r="R40" s="28"/>
-      <c r="S40" s="28"/>
-      <c r="T40" s="28"/>
-      <c r="U40" s="28"/>
-      <c r="V40" s="28"/>
-      <c r="W40" s="28"/>
-      <c r="X40" s="28"/>
-      <c r="Y40" s="28"/>
-      <c r="Z40" s="28"/>
-      <c r="AA40" s="28"/>
-      <c r="AB40" s="28"/>
-      <c r="AC40" s="28"/>
-      <c r="AD40" s="28"/>
-      <c r="AE40" s="28"/>
-      <c r="AF40" s="28"/>
-      <c r="AG40" s="28"/>
-      <c r="AH40" s="28"/>
-      <c r="AI40" s="28"/>
-      <c r="AJ40" s="28"/>
-      <c r="AK40" s="28"/>
-      <c r="AL40" s="28"/>
-      <c r="AM40" s="28"/>
-      <c r="AN40" s="28"/>
-      <c r="AO40" s="28"/>
-      <c r="AP40" s="28"/>
-      <c r="AQ40" s="28"/>
-      <c r="AR40" s="28"/>
-      <c r="AS40" s="28"/>
-      <c r="AT40" s="28"/>
-      <c r="AU40" s="28"/>
-      <c r="AV40" s="28"/>
-      <c r="AW40" s="28"/>
-      <c r="AX40" s="28"/>
-      <c r="AY40" s="28"/>
-      <c r="AZ40" s="28"/>
-      <c r="BA40" s="28"/>
-      <c r="BB40" s="28"/>
-      <c r="BC40" s="28"/>
-      <c r="BD40" s="28"/>
-      <c r="BE40" s="28"/>
-      <c r="BF40" s="28"/>
-      <c r="BG40" s="28"/>
-      <c r="BH40" s="28"/>
-      <c r="BI40" s="28"/>
-      <c r="BJ40" s="28"/>
-      <c r="BK40" s="28"/>
-      <c r="BL40" s="28"/>
-      <c r="BM40" s="28"/>
-      <c r="BN40" s="28"/>
-      <c r="BO40" s="28"/>
-      <c r="BP40" s="28"/>
-      <c r="BQ40" s="28"/>
-      <c r="BR40" s="28"/>
-      <c r="BS40" s="28"/>
-      <c r="BT40" s="28"/>
-      <c r="BU40" s="28"/>
-      <c r="BV40" s="28"/>
-      <c r="BW40" s="28"/>
-      <c r="BX40" s="28"/>
-      <c r="BY40" s="28"/>
+      <c r="H39" s="28"/>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="28"/>
+      <c r="P39" s="28"/>
+      <c r="Q39" s="28"/>
+      <c r="R39" s="28"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="28"/>
+      <c r="V39" s="28"/>
+      <c r="W39" s="28"/>
+      <c r="X39" s="28"/>
+      <c r="Y39" s="28"/>
+      <c r="Z39" s="28"/>
+      <c r="AA39" s="28"/>
+      <c r="AB39" s="28"/>
+      <c r="AC39" s="28"/>
+      <c r="AD39" s="28"/>
+      <c r="AE39" s="28"/>
+      <c r="AF39" s="28"/>
+      <c r="AG39" s="28"/>
+      <c r="AH39" s="28"/>
+      <c r="AI39" s="28"/>
+      <c r="AJ39" s="28"/>
+      <c r="AK39" s="28"/>
+      <c r="AL39" s="28"/>
+      <c r="AM39" s="28"/>
+      <c r="AN39" s="28"/>
+      <c r="AO39" s="28"/>
+      <c r="AP39" s="28"/>
+      <c r="AQ39" s="28"/>
+      <c r="AR39" s="28"/>
+      <c r="AS39" s="28"/>
+      <c r="AT39" s="28"/>
+      <c r="AU39" s="28"/>
+      <c r="AV39" s="28"/>
+      <c r="AW39" s="28"/>
+      <c r="AX39" s="28"/>
+      <c r="AY39" s="28"/>
+      <c r="AZ39" s="28"/>
+      <c r="BA39" s="28"/>
+      <c r="BB39" s="28"/>
+      <c r="BC39" s="28"/>
+      <c r="BD39" s="28"/>
+      <c r="BE39" s="28"/>
+      <c r="BF39" s="28"/>
+      <c r="BG39" s="28"/>
+      <c r="BH39" s="28"/>
+      <c r="BI39" s="28"/>
+      <c r="BJ39" s="28"/>
+      <c r="BK39" s="28"/>
+      <c r="BL39" s="28"/>
+      <c r="BM39" s="28"/>
+      <c r="BN39" s="28"/>
+      <c r="BO39" s="28"/>
+      <c r="BP39" s="28"/>
+      <c r="BQ39" s="28"/>
+      <c r="BR39" s="28"/>
+      <c r="BS39" s="28"/>
+      <c r="BT39" s="28"/>
+      <c r="BU39" s="28"/>
+      <c r="BV39" s="28"/>
+      <c r="BW39" s="28"/>
+      <c r="BX39" s="28"/>
+      <c r="BY39" s="28"/>
+    </row>
+    <row r="40" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E42" s="42"/>
+      <c r="E41" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5813,7 +5669,7 @@
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C40">
+  <conditionalFormatting sqref="C7:C39">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5827,49 +5683,29 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BJ40">
-    <cfRule type="expression" dxfId="8" priority="39">
+  <conditionalFormatting sqref="H5:BJ39 BL5:BQ39 BS5:BX39">
+    <cfRule type="expression" dxfId="4" priority="39">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BJ40">
-    <cfRule type="expression" dxfId="7" priority="34" stopIfTrue="1">
+  <conditionalFormatting sqref="H7:BJ39 BL7:BQ39 BS7:BX39">
+    <cfRule type="expression" dxfId="3" priority="34" stopIfTrue="1">
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BY40">
-    <cfRule type="expression" dxfId="6" priority="1">
+  <conditionalFormatting sqref="H7:BY39">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK5:BK40 BR5:BR40 BY5:BY40">
-    <cfRule type="expression" dxfId="5" priority="41">
+  <conditionalFormatting sqref="BK5:BK39 BR5:BR39 BY5:BY39">
+    <cfRule type="expression" dxfId="1" priority="41">
       <formula>AND(TODAY()&gt;=BK$5,TODAY()&lt;BZ$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK7:BK40 BR7:BR40 BY7:BY40">
-    <cfRule type="expression" dxfId="4" priority="45" stopIfTrue="1">
+  <conditionalFormatting sqref="BK7:BK39 BR7:BR39 BY7:BY39">
+    <cfRule type="expression" dxfId="0" priority="45" stopIfTrue="1">
       <formula>AND(task_end&gt;=BK$5,task_start&lt;BZ$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BL5:BQ40">
-    <cfRule type="expression" dxfId="3" priority="6">
-      <formula>AND(TODAY()&gt;=BL$5,TODAY()&lt;BM$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BL7:BQ40">
-    <cfRule type="expression" dxfId="2" priority="5" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BL$5,task_start&lt;BM$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BS5:BX40">
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>AND(TODAY()&gt;=BS$5,TODAY()&lt;BT$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BS7:BX40">
-    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
-      <formula>AND(task_end&gt;=BS$5,task_start&lt;BT$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5906,7 +5742,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C40</xm:sqref>
+          <xm:sqref>C7:C39</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5929,79 +5765,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:2" s="36" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="37"/>
     </row>
     <row r="4" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="30" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -6018,6 +5854,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6305,36 +6170,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6353,24 +6209,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TFG: Documentation previous to the app development finished
</commit_message>
<xml_diff>
--- a/TFG/TFG Diagrama de Gantt.xlsx
+++ b/TFG/TFG Diagrama de Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536AC0F-BA09-524A-B34A-FC3B63F1811D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BCA460-C766-4542-B668-4BDDCD876AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -204,9 +204,6 @@
   </si>
   <si>
     <t>Hola</t>
-  </si>
-  <si>
-    <t>Insertado</t>
   </si>
   <si>
     <t>Ofimática</t>
@@ -307,22 +304,28 @@
     <t>Conexión de la API privada con el front-end</t>
   </si>
   <si>
-    <t>Inserción de ejercicios</t>
-  </si>
-  <si>
     <t>Diagrama de casos de uso</t>
   </si>
   <si>
-    <t>Formación: Swift</t>
-  </si>
-  <si>
-    <t>Formación: SwiftUI</t>
-  </si>
-  <si>
     <t>CRUD básico</t>
   </si>
   <si>
     <t>Estructura por capas</t>
+  </si>
+  <si>
+    <t>Inserción de datos</t>
+  </si>
+  <si>
+    <t>Segunda formación: SwiftUI</t>
+  </si>
+  <si>
+    <t>Primera Formación: SwiftUI</t>
+  </si>
+  <si>
+    <t>Tercera formación: Swift</t>
+  </si>
+  <si>
+    <t>Testing de la aplicación</t>
   </si>
 </sst>
 </file>
@@ -2014,7 +2017,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2035,7 +2038,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
@@ -2060,7 +2063,7 @@
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" s="80">
         <v>45719</v>
@@ -2852,7 +2855,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="55"/>
@@ -2938,7 +2941,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -3031,7 +3034,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
@@ -3123,7 +3126,7 @@
     <row r="11" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="13">
         <v>1</v>
@@ -3214,7 +3217,7 @@
     <row r="12" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" s="13">
         <v>1</v>
@@ -3304,13 +3307,13 @@
     <row r="13" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C13" s="13">
         <v>0.2</v>
       </c>
       <c r="D13" s="57">
-        <v>45722</v>
+        <v>45727</v>
       </c>
       <c r="E13" s="57">
         <v>45730</v>
@@ -3391,9 +3394,11 @@
     <row r="14" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="46" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="13"/>
+        <v>55</v>
+      </c>
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
       <c r="D14" s="57">
         <v>45732</v>
       </c>
@@ -3476,9 +3481,11 @@
     <row r="15" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="73" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="13"/>
+        <v>48</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
       <c r="D15" s="57">
         <v>45736</v>
       </c>
@@ -3640,21 +3647,19 @@
     <row r="17" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="40"/>
       <c r="B17" s="46" t="s">
-        <v>16</v>
+        <v>62</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="57">
-        <f>D10+1</f>
-        <v>45721</v>
+        <v>45778</v>
       </c>
       <c r="E17" s="57">
-        <f>D17+2</f>
-        <v>45723</v>
+        <v>45791</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
@@ -3816,10 +3821,10 @@
     <row r="19" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41"/>
       <c r="B19" s="47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="16">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D19" s="60">
         <v>45735</v>
@@ -3906,7 +3911,7 @@
     <row r="20" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="47" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="16">
         <v>1</v>
@@ -3996,9 +4001,11 @@
     <row r="21" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="16"/>
+        <v>58</v>
+      </c>
+      <c r="C21" s="16">
+        <v>1</v>
+      </c>
       <c r="D21" s="60">
         <v>45742</v>
       </c>
@@ -4087,18 +4094,12 @@
         <v>15</v>
       </c>
       <c r="C22" s="16"/>
-      <c r="D22" s="60">
-        <f>D21</f>
-        <v>45742</v>
-      </c>
-      <c r="E22" s="60">
-        <f>D22+2</f>
-        <v>45744</v>
-      </c>
+      <c r="D22" s="60"/>
+      <c r="E22" s="60"/>
       <c r="F22" s="10"/>
-      <c r="G22" s="10">
+      <c r="G22" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v/>
       </c>
       <c r="H22" s="26"/>
       <c r="I22" s="26"/>
@@ -4177,18 +4178,12 @@
         <v>16</v>
       </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="60">
-        <f>D22</f>
-        <v>45742</v>
-      </c>
-      <c r="E23" s="60">
-        <f>D23+3</f>
-        <v>45745</v>
-      </c>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
       <c r="F23" s="10"/>
-      <c r="G23" s="10">
+      <c r="G23" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v/>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
@@ -4350,21 +4345,15 @@
     <row r="25" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="48" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" s="19"/>
-      <c r="D25" s="63">
-        <f>D9+15</f>
-        <v>45734</v>
-      </c>
-      <c r="E25" s="63">
-        <f>D25+5</f>
-        <v>45739</v>
-      </c>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
       <c r="F25" s="10"/>
-      <c r="G25" s="10">
+      <c r="G25" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>6</v>
+        <v/>
       </c>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
@@ -4440,19 +4429,15 @@
     <row r="26" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="48" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C26" s="19"/>
-      <c r="D26" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="63" t="s">
-        <v>20</v>
-      </c>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
       <c r="F26" s="10"/>
-      <c r="G26" s="10" t="e">
+      <c r="G26" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
@@ -4528,19 +4513,15 @@
     <row r="27" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="48" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C27" s="19"/>
-      <c r="D27" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="63" t="s">
-        <v>20</v>
-      </c>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
       <c r="F27" s="10"/>
-      <c r="G27" s="10" t="e">
+      <c r="G27" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
@@ -4617,16 +4598,12 @@
       <c r="A28" s="40"/>
       <c r="B28" s="48"/>
       <c r="C28" s="19"/>
-      <c r="D28" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="63" t="s">
-        <v>20</v>
-      </c>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
       <c r="F28" s="10"/>
-      <c r="G28" s="10" t="e">
+      <c r="G28" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
@@ -4860,7 +4837,7 @@
     <row r="31" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C31" s="19"/>
       <c r="D31" s="63" t="s">
@@ -5034,7 +5011,7 @@
     <row r="33" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="49" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="22">
         <v>1</v>
@@ -5124,7 +5101,7 @@
     <row r="34" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="49" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C34" s="22">
         <v>1</v>
@@ -5214,19 +5191,21 @@
     <row r="35" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="49" t="s">
-        <v>15</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="E35" s="66" t="s">
-        <v>20</v>
+        <v>61</v>
+      </c>
+      <c r="C35" s="22">
+        <v>0.6</v>
+      </c>
+      <c r="D35" s="66">
+        <v>45741</v>
+      </c>
+      <c r="E35" s="66">
+        <v>45750</v>
       </c>
       <c r="F35" s="10"/>
-      <c r="G35" s="10" t="e">
+      <c r="G35" s="10">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v>10</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -5301,16 +5280,10 @@
     </row>
     <row r="36" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
-      <c r="B36" s="49" t="s">
-        <v>42</v>
-      </c>
+      <c r="B36" s="49"/>
       <c r="C36" s="22"/>
-      <c r="D36" s="66">
-        <v>45778</v>
-      </c>
-      <c r="E36" s="66">
-        <v>45779</v>
-      </c>
+      <c r="D36" s="66"/>
+      <c r="E36" s="66"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="26"/>
@@ -5386,20 +5359,14 @@
     </row>
     <row r="37" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
-      <c r="B37" s="49" t="s">
-        <v>16</v>
-      </c>
+      <c r="B37" s="49"/>
       <c r="C37" s="22"/>
-      <c r="D37" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="66" t="s">
-        <v>20</v>
-      </c>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
       <c r="F37" s="10"/>
-      <c r="G37" s="10" t="e">
+      <c r="G37" s="10" t="str">
         <f t="shared" si="18"/>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -5723,9 +5690,6 @@
   <headerFooter differentFirst="1" scaleWithDoc="0">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <ignoredErrors>
-    <ignoredError sqref="E22" formula="1"/>
-  </ignoredErrors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -5854,35 +5818,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6170,27 +6105,36 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6209,4 +6153,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TFG: Documentation- Arrived at the domain packet explanation
</commit_message>
<xml_diff>
--- a/TFG/TFG Diagrama de Gantt.xlsx
+++ b/TFG/TFG Diagrama de Gantt.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9BCA460-C766-4542-B668-4BDDCD876AA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB732B4B-5277-5446-85C2-388E8F72156A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
   <si>
     <t>Cree una programación para un proyecto en esta hoja de cálculo.
 Escriba el título de este proyecto en la celda B1. 
@@ -120,12 +120,6 @@
     <t>TAREA</t>
   </si>
   <si>
-    <t>Tarea 4</t>
-  </si>
-  <si>
-    <t>Tarea 5</t>
-  </si>
-  <si>
     <t>Inserte nuevas filas ENCIMA de ésta</t>
   </si>
   <si>
@@ -133,9 +127,6 @@
   </si>
   <si>
     <t>INICIO</t>
-  </si>
-  <si>
-    <t>fecha</t>
   </si>
   <si>
     <t>FIN</t>
@@ -298,18 +289,9 @@
     <t>Creación de tablas de base de datos en MariaDB</t>
   </si>
   <si>
-    <t>Aprendizaje de JWT (JSON Web Token)</t>
-  </si>
-  <si>
-    <t>Conexión de la API privada con el front-end</t>
-  </si>
-  <si>
     <t>Diagrama de casos de uso</t>
   </si>
   <si>
-    <t>CRUD básico</t>
-  </si>
-  <si>
     <t>Estructura por capas</t>
   </si>
   <si>
@@ -325,7 +307,55 @@
     <t>Tercera formación: Swift</t>
   </si>
   <si>
-    <t>Testing de la aplicación</t>
+    <t>Fix en el orden de creación de las tablas para automatizar</t>
+  </si>
+  <si>
+    <t>CORS</t>
+  </si>
+  <si>
+    <t>CRUD básico Exercises</t>
+  </si>
+  <si>
+    <t>CRUD básico Sessions</t>
+  </si>
+  <si>
+    <t>CRUD básico Trainings</t>
+  </si>
+  <si>
+    <t>CRUD básico Users</t>
+  </si>
+  <si>
+    <t>CRUD básico SessionsTrainings</t>
+  </si>
+  <si>
+    <t>CRUD básico ExerciseTypes &amp; ExerciseSubtypes</t>
+  </si>
+  <si>
+    <t>Cuarta formación: arquitecturas Swift y SwiftUI</t>
+  </si>
+  <si>
+    <t>Configuración global aplicación</t>
+  </si>
+  <si>
+    <t>4-31-25</t>
+  </si>
+  <si>
+    <t>Vistas módulo User</t>
+  </si>
+  <si>
+    <t>Vistas módulo Exercises</t>
+  </si>
+  <si>
+    <t>Vistas módulo Sessions</t>
+  </si>
+  <si>
+    <t>Vistas módulo Trainings</t>
+  </si>
+  <si>
+    <t>Checkeo con el back-end</t>
+  </si>
+  <si>
+    <t>Application Properties</t>
   </si>
 </sst>
 </file>
@@ -333,10 +363,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="8">
-    <numFmt numFmtId="42" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0\ &quot;€&quot;_-;\-* #,##0\ &quot;€&quot;_-;_-* &quot;-&quot;\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="d\-m\-yy;@"/>
     <numFmt numFmtId="167" formatCode="d"/>
     <numFmt numFmtId="168" formatCode="ddd\,\ yyyy\-mm\-dd;@"/>
@@ -1090,7 +1120,7 @@
     </xf>
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="3" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -1112,9 +1142,9 @@
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1433,7 +1463,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Note" xfId="27" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="22" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Per cent" xfId="2" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5" customBuiltin="1"/>
     <cellStyle name="Tarea" xfId="12" xr:uid="{6391D789-272B-4DD2-9BF3-2CDCF610FA41}"/>
     <cellStyle name="Title" xfId="5" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="29" builtinId="25" customBuiltin="1"/>
@@ -2013,11 +2043,11 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BY41"/>
+  <dimension ref="A1:BY47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O38" sqref="O38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2038,14 +2068,14 @@
         <v>0</v>
       </c>
       <c r="B1" s="43" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="3"/>
       <c r="E1" s="29"/>
       <c r="G1" s="1"/>
       <c r="H1" s="52" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2054,7 +2084,7 @@
       </c>
       <c r="B2" s="44"/>
       <c r="H2" s="53" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2063,7 +2093,7 @@
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="76" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D3" s="80">
         <v>45719</v>
@@ -2477,17 +2507,17 @@
         <v>14</v>
       </c>
       <c r="C6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>21</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H6" s="8" t="str">
         <f t="shared" ref="H6" si="13">LEFT(TEXT(H5,"ddd"),1)</f>
@@ -2855,14 +2885,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="55"/>
       <c r="E8" s="56"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10" t="str">
-        <f t="shared" ref="G8:G39" si="18">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="G8:G45" si="18">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="H8" s="26"/>
@@ -2941,7 +2971,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C9" s="13">
         <v>1</v>
@@ -3034,7 +3064,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C10" s="13">
         <v>1</v>
@@ -3126,7 +3156,7 @@
     <row r="11" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="40"/>
       <c r="B11" s="46" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="13">
         <v>1</v>
@@ -3217,7 +3247,7 @@
     <row r="12" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="40"/>
       <c r="B12" s="46" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="13">
         <v>1</v>
@@ -3307,10 +3337,10 @@
     <row r="13" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="40"/>
       <c r="B13" s="46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="13">
-        <v>0.2</v>
+        <v>1</v>
       </c>
       <c r="D13" s="57">
         <v>45727</v>
@@ -3394,7 +3424,7 @@
     <row r="14" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40"/>
       <c r="B14" s="46" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C14" s="13">
         <v>1</v>
@@ -3481,7 +3511,7 @@
     <row r="15" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="40"/>
       <c r="B15" s="73" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15" s="13">
         <v>1</v>
@@ -3566,13 +3596,20 @@
       <c r="BY15" s="26"/>
     </row>
     <row r="16" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="73"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
+      <c r="A16" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
+      <c r="G16" s="10" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
       <c r="H16" s="26"/>
       <c r="I16" s="26"/>
       <c r="J16" s="26"/>
@@ -3589,7 +3626,7 @@
       <c r="U16" s="26"/>
       <c r="V16" s="26"/>
       <c r="W16" s="26"/>
-      <c r="X16" s="27"/>
+      <c r="X16" s="26"/>
       <c r="Y16" s="26"/>
       <c r="Z16" s="26"/>
       <c r="AA16" s="26"/>
@@ -3645,21 +3682,23 @@
       <c r="BY16" s="26"/>
     </row>
     <row r="17" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="57">
-        <v>45778</v>
-      </c>
-      <c r="E17" s="57">
-        <v>45791</v>
+      <c r="A17" s="41"/>
+      <c r="B17" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="60">
+        <v>45735</v>
+      </c>
+      <c r="E17" s="60">
+        <v>45737</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10">
         <f t="shared" si="18"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="H17" s="26"/>
       <c r="I17" s="26"/>
@@ -3733,19 +3772,23 @@
       <c r="BY17" s="26"/>
     </row>
     <row r="18" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="59"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="60">
+        <v>45738</v>
+      </c>
+      <c r="E18" s="60">
+        <v>45741</v>
+      </c>
       <c r="F18" s="10"/>
-      <c r="G18" s="10" t="str">
+      <c r="G18" s="10">
         <f t="shared" si="18"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="H18" s="26"/>
       <c r="I18" s="26"/>
@@ -3759,8 +3802,8 @@
       <c r="Q18" s="26"/>
       <c r="R18" s="26"/>
       <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
+      <c r="T18" s="27"/>
+      <c r="U18" s="27"/>
       <c r="V18" s="26"/>
       <c r="W18" s="26"/>
       <c r="X18" s="26"/>
@@ -3819,23 +3862,23 @@
       <c r="BY18" s="26"/>
     </row>
     <row r="19" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="40"/>
       <c r="B19" s="47" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="16">
         <v>1</v>
       </c>
       <c r="D19" s="60">
-        <v>45735</v>
+        <v>45742</v>
       </c>
       <c r="E19" s="60">
-        <v>45737</v>
+        <v>45746</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10">
         <f t="shared" si="18"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H19" s="26"/>
       <c r="I19" s="26"/>
@@ -3911,21 +3954,21 @@
     <row r="20" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="47" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C20" s="16">
         <v>1</v>
       </c>
       <c r="D20" s="60">
-        <v>45738</v>
+        <v>45761</v>
       </c>
       <c r="E20" s="60">
-        <v>45741</v>
+        <v>45765</v>
       </c>
       <c r="F20" s="10"/>
       <c r="G20" s="10">
         <f t="shared" si="18"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H20" s="26"/>
       <c r="I20" s="26"/>
@@ -3939,11 +3982,11 @@
       <c r="Q20" s="26"/>
       <c r="R20" s="26"/>
       <c r="S20" s="26"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
       <c r="V20" s="26"/>
       <c r="W20" s="26"/>
-      <c r="X20" s="26"/>
+      <c r="X20" s="27"/>
       <c r="Y20" s="26"/>
       <c r="Z20" s="26"/>
       <c r="AA20" s="26"/>
@@ -4001,21 +4044,21 @@
     <row r="21" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="47" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C21" s="16">
         <v>1</v>
       </c>
       <c r="D21" s="60">
-        <v>45742</v>
+        <v>45769</v>
       </c>
       <c r="E21" s="60">
-        <v>45746</v>
+        <v>45772</v>
       </c>
       <c r="F21" s="10"/>
       <c r="G21" s="10">
         <f t="shared" si="18"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H21" s="26"/>
       <c r="I21" s="26"/>
@@ -4089,13 +4132,15 @@
       <c r="BY21" s="26"/>
     </row>
     <row r="22" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="47" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
+      <c r="A22" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="62"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="str">
         <f t="shared" si="18"/>
@@ -4117,7 +4162,7 @@
       <c r="U22" s="26"/>
       <c r="V22" s="26"/>
       <c r="W22" s="26"/>
-      <c r="X22" s="27"/>
+      <c r="X22" s="26"/>
       <c r="Y22" s="26"/>
       <c r="Z22" s="26"/>
       <c r="AA22" s="26"/>
@@ -4174,16 +4219,22 @@
     </row>
     <row r="23" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="40"/>
-      <c r="B23" s="47" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
+      <c r="B23" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="19">
+        <v>1</v>
+      </c>
+      <c r="D23" s="63">
+        <v>45754</v>
+      </c>
+      <c r="E23" s="63">
+        <v>45757</v>
+      </c>
       <c r="F23" s="10"/>
-      <c r="G23" s="10" t="str">
+      <c r="G23" s="10">
         <f t="shared" si="18"/>
-        <v/>
+        <v>4</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="26"/>
@@ -4257,20 +4308,21 @@
       <c r="BY23" s="26"/>
     </row>
     <row r="24" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
-        <v>11</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="18"/>
-      <c r="D24" s="61"/>
-      <c r="E24" s="62"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="19">
+        <v>1</v>
+      </c>
+      <c r="D24" s="63">
+        <v>45754</v>
+      </c>
+      <c r="E24" s="63">
+        <v>45755</v>
+      </c>
       <c r="F24" s="10"/>
-      <c r="G24" s="10" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
+      <c r="G24" s="10"/>
       <c r="H24" s="26"/>
       <c r="I24" s="26"/>
       <c r="J24" s="26"/>
@@ -4345,16 +4397,19 @@
     <row r="25" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40"/>
       <c r="B25" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="19"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
+        <v>72</v>
+      </c>
+      <c r="C25" s="19">
+        <v>1</v>
+      </c>
+      <c r="D25" s="63">
+        <v>45756</v>
+      </c>
+      <c r="E25" s="63">
+        <v>45757</v>
+      </c>
       <c r="F25" s="10"/>
-      <c r="G25" s="10" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
+      <c r="G25" s="10"/>
       <c r="H25" s="26"/>
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
@@ -4429,16 +4484,19 @@
     <row r="26" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="40"/>
       <c r="B26" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
+        <v>61</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+      <c r="D26" s="63">
+        <v>45758</v>
+      </c>
+      <c r="E26" s="63">
+        <v>45759</v>
+      </c>
       <c r="F26" s="10"/>
-      <c r="G26" s="10" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
+      <c r="G26" s="10"/>
       <c r="H26" s="26"/>
       <c r="I26" s="26"/>
       <c r="J26" s="26"/>
@@ -4513,15 +4571,21 @@
     <row r="27" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="40"/>
       <c r="B27" s="48" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
+        <v>58</v>
+      </c>
+      <c r="C27" s="19">
+        <v>1</v>
+      </c>
+      <c r="D27" s="63">
+        <v>45761</v>
+      </c>
+      <c r="E27" s="63">
+        <v>45763</v>
+      </c>
       <c r="F27" s="10"/>
-      <c r="G27" s="10" t="str">
+      <c r="G27" s="10">
         <f t="shared" si="18"/>
-        <v/>
+        <v>3</v>
       </c>
       <c r="H27" s="26"/>
       <c r="I27" s="26"/>
@@ -4596,15 +4660,20 @@
     </row>
     <row r="28" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
+      <c r="B28" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="19">
+        <v>1</v>
+      </c>
+      <c r="D28" s="63">
+        <v>45761</v>
+      </c>
+      <c r="E28" s="63">
+        <v>45763</v>
+      </c>
       <c r="F28" s="10"/>
-      <c r="G28" s="10" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
+      <c r="G28" s="10"/>
       <c r="H28" s="26"/>
       <c r="I28" s="26"/>
       <c r="J28" s="26"/>
@@ -4678,12 +4747,23 @@
     </row>
     <row r="29" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="40"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
+      <c r="B29" s="48" t="s">
+        <v>59</v>
+      </c>
+      <c r="C29" s="19">
+        <v>1</v>
+      </c>
+      <c r="D29" s="63">
+        <v>45766</v>
+      </c>
+      <c r="E29" s="63">
+        <v>45768</v>
+      </c>
       <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
+      <c r="G29" s="10">
+        <f t="shared" si="18"/>
+        <v>3</v>
+      </c>
       <c r="H29" s="26"/>
       <c r="I29" s="26"/>
       <c r="J29" s="26"/>
@@ -4757,10 +4837,18 @@
     </row>
     <row r="30" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="40"/>
-      <c r="B30" s="48"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
+      <c r="B30" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" s="19">
+        <v>1</v>
+      </c>
+      <c r="D30" s="63">
+        <v>45769</v>
+      </c>
+      <c r="E30" s="63">
+        <v>45771</v>
+      </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="26"/>
@@ -4837,20 +4925,19 @@
     <row r="31" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="40"/>
       <c r="B31" s="48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="63" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="63" t="s">
-        <v>20</v>
+        <v>62</v>
+      </c>
+      <c r="C31" s="19">
+        <v>1</v>
+      </c>
+      <c r="D31" s="63">
+        <v>45772</v>
+      </c>
+      <c r="E31" s="63">
+        <v>45775</v>
       </c>
       <c r="F31" s="10"/>
-      <c r="G31" s="10" t="e">
-        <f t="shared" si="18"/>
-        <v>#VALUE!</v>
-      </c>
+      <c r="G31" s="10"/>
       <c r="H31" s="26"/>
       <c r="I31" s="26"/>
       <c r="J31" s="26"/>
@@ -4927,7 +5014,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C32" s="21"/>
       <c r="D32" s="64"/>
@@ -5011,7 +5098,7 @@
     <row r="33" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="40"/>
       <c r="B33" s="49" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C33" s="22">
         <v>1</v>
@@ -5101,7 +5188,7 @@
     <row r="34" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="40"/>
       <c r="B34" s="49" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C34" s="22">
         <v>1</v>
@@ -5191,10 +5278,10 @@
     <row r="35" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="40"/>
       <c r="B35" s="49" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C35" s="22">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="D35" s="66">
         <v>45741</v>
@@ -5280,10 +5367,18 @@
     </row>
     <row r="36" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="40"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="22"/>
-      <c r="D36" s="66"/>
-      <c r="E36" s="66"/>
+      <c r="B36" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="22">
+        <v>1</v>
+      </c>
+      <c r="D36" s="66">
+        <v>45751</v>
+      </c>
+      <c r="E36" s="66">
+        <v>45758</v>
+      </c>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="26"/>
@@ -5359,15 +5454,20 @@
     </row>
     <row r="37" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="40"/>
-      <c r="B37" s="49"/>
-      <c r="C37" s="22"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
+      <c r="B37" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="22">
+        <v>0</v>
+      </c>
+      <c r="D37" s="66">
+        <v>45776</v>
+      </c>
+      <c r="E37" s="66" t="s">
+        <v>66</v>
+      </c>
       <c r="F37" s="10"/>
-      <c r="G37" s="10" t="str">
-        <f t="shared" si="18"/>
-        <v/>
-      </c>
+      <c r="G37" s="10"/>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
       <c r="J37" s="26"/>
@@ -5440,25 +5540,17 @@
       <c r="BY37" s="26"/>
     </row>
     <row r="38" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="B38" s="50" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="9"/>
-      <c r="D38" s="67">
-        <v>45782</v>
-      </c>
-      <c r="E38" s="67">
-        <f>D38+5</f>
-        <v>45787</v>
-      </c>
+      <c r="A38" s="40"/>
+      <c r="B38" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="22">
+        <v>0</v>
+      </c>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
       <c r="F38" s="10"/>
-      <c r="G38" s="10">
-        <f t="shared" si="18"/>
-        <v>6</v>
-      </c>
+      <c r="G38" s="10"/>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
@@ -5531,96 +5623,595 @@
       <c r="BY38" s="26"/>
     </row>
     <row r="39" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B39" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C39" s="24"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="69"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25" t="str">
+      <c r="A39" s="40"/>
+      <c r="B39" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="22">
+        <v>0</v>
+      </c>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="26"/>
+      <c r="I39" s="26"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="26"/>
+      <c r="L39" s="26"/>
+      <c r="M39" s="26"/>
+      <c r="N39" s="26"/>
+      <c r="O39" s="26"/>
+      <c r="P39" s="26"/>
+      <c r="Q39" s="26"/>
+      <c r="R39" s="26"/>
+      <c r="S39" s="26"/>
+      <c r="T39" s="26"/>
+      <c r="U39" s="26"/>
+      <c r="V39" s="26"/>
+      <c r="W39" s="26"/>
+      <c r="X39" s="26"/>
+      <c r="Y39" s="26"/>
+      <c r="Z39" s="26"/>
+      <c r="AA39" s="26"/>
+      <c r="AB39" s="26"/>
+      <c r="AC39" s="26"/>
+      <c r="AD39" s="26"/>
+      <c r="AE39" s="26"/>
+      <c r="AF39" s="26"/>
+      <c r="AG39" s="26"/>
+      <c r="AH39" s="26"/>
+      <c r="AI39" s="26"/>
+      <c r="AJ39" s="26"/>
+      <c r="AK39" s="26"/>
+      <c r="AL39" s="26"/>
+      <c r="AM39" s="26"/>
+      <c r="AN39" s="26"/>
+      <c r="AO39" s="26"/>
+      <c r="AP39" s="26"/>
+      <c r="AQ39" s="26"/>
+      <c r="AR39" s="26"/>
+      <c r="AS39" s="26"/>
+      <c r="AT39" s="26"/>
+      <c r="AU39" s="26"/>
+      <c r="AV39" s="26"/>
+      <c r="AW39" s="26"/>
+      <c r="AX39" s="26"/>
+      <c r="AY39" s="26"/>
+      <c r="AZ39" s="26"/>
+      <c r="BA39" s="26"/>
+      <c r="BB39" s="26"/>
+      <c r="BC39" s="26"/>
+      <c r="BD39" s="26"/>
+      <c r="BE39" s="26"/>
+      <c r="BF39" s="26"/>
+      <c r="BG39" s="26"/>
+      <c r="BH39" s="26"/>
+      <c r="BI39" s="26"/>
+      <c r="BJ39" s="26"/>
+      <c r="BK39" s="26"/>
+      <c r="BL39" s="26"/>
+      <c r="BM39" s="26"/>
+      <c r="BN39" s="26"/>
+      <c r="BO39" s="26"/>
+      <c r="BP39" s="26"/>
+      <c r="BQ39" s="26"/>
+      <c r="BR39" s="26"/>
+      <c r="BS39" s="26"/>
+      <c r="BT39" s="26"/>
+      <c r="BU39" s="26"/>
+      <c r="BV39" s="26"/>
+      <c r="BW39" s="26"/>
+      <c r="BX39" s="26"/>
+      <c r="BY39" s="26"/>
+    </row>
+    <row r="40" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="40"/>
+      <c r="B40" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="22">
+        <v>0</v>
+      </c>
+      <c r="D40" s="66"/>
+      <c r="E40" s="66"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="26"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="26"/>
+      <c r="K40" s="26"/>
+      <c r="L40" s="26"/>
+      <c r="M40" s="26"/>
+      <c r="N40" s="26"/>
+      <c r="O40" s="26"/>
+      <c r="P40" s="26"/>
+      <c r="Q40" s="26"/>
+      <c r="R40" s="26"/>
+      <c r="S40" s="26"/>
+      <c r="T40" s="26"/>
+      <c r="U40" s="26"/>
+      <c r="V40" s="26"/>
+      <c r="W40" s="26"/>
+      <c r="X40" s="26"/>
+      <c r="Y40" s="26"/>
+      <c r="Z40" s="26"/>
+      <c r="AA40" s="26"/>
+      <c r="AB40" s="26"/>
+      <c r="AC40" s="26"/>
+      <c r="AD40" s="26"/>
+      <c r="AE40" s="26"/>
+      <c r="AF40" s="26"/>
+      <c r="AG40" s="26"/>
+      <c r="AH40" s="26"/>
+      <c r="AI40" s="26"/>
+      <c r="AJ40" s="26"/>
+      <c r="AK40" s="26"/>
+      <c r="AL40" s="26"/>
+      <c r="AM40" s="26"/>
+      <c r="AN40" s="26"/>
+      <c r="AO40" s="26"/>
+      <c r="AP40" s="26"/>
+      <c r="AQ40" s="26"/>
+      <c r="AR40" s="26"/>
+      <c r="AS40" s="26"/>
+      <c r="AT40" s="26"/>
+      <c r="AU40" s="26"/>
+      <c r="AV40" s="26"/>
+      <c r="AW40" s="26"/>
+      <c r="AX40" s="26"/>
+      <c r="AY40" s="26"/>
+      <c r="AZ40" s="26"/>
+      <c r="BA40" s="26"/>
+      <c r="BB40" s="26"/>
+      <c r="BC40" s="26"/>
+      <c r="BD40" s="26"/>
+      <c r="BE40" s="26"/>
+      <c r="BF40" s="26"/>
+      <c r="BG40" s="26"/>
+      <c r="BH40" s="26"/>
+      <c r="BI40" s="26"/>
+      <c r="BJ40" s="26"/>
+      <c r="BK40" s="26"/>
+      <c r="BL40" s="26"/>
+      <c r="BM40" s="26"/>
+      <c r="BN40" s="26"/>
+      <c r="BO40" s="26"/>
+      <c r="BP40" s="26"/>
+      <c r="BQ40" s="26"/>
+      <c r="BR40" s="26"/>
+      <c r="BS40" s="26"/>
+      <c r="BT40" s="26"/>
+      <c r="BU40" s="26"/>
+      <c r="BV40" s="26"/>
+      <c r="BW40" s="26"/>
+      <c r="BX40" s="26"/>
+      <c r="BY40" s="26"/>
+    </row>
+    <row r="41" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="40"/>
+      <c r="B41" s="49" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="26"/>
+      <c r="I41" s="26"/>
+      <c r="J41" s="26"/>
+      <c r="K41" s="26"/>
+      <c r="L41" s="26"/>
+      <c r="M41" s="26"/>
+      <c r="N41" s="26"/>
+      <c r="O41" s="26"/>
+      <c r="P41" s="26"/>
+      <c r="Q41" s="26"/>
+      <c r="R41" s="26"/>
+      <c r="S41" s="26"/>
+      <c r="T41" s="26"/>
+      <c r="U41" s="26"/>
+      <c r="V41" s="26"/>
+      <c r="W41" s="26"/>
+      <c r="X41" s="26"/>
+      <c r="Y41" s="26"/>
+      <c r="Z41" s="26"/>
+      <c r="AA41" s="26"/>
+      <c r="AB41" s="26"/>
+      <c r="AC41" s="26"/>
+      <c r="AD41" s="26"/>
+      <c r="AE41" s="26"/>
+      <c r="AF41" s="26"/>
+      <c r="AG41" s="26"/>
+      <c r="AH41" s="26"/>
+      <c r="AI41" s="26"/>
+      <c r="AJ41" s="26"/>
+      <c r="AK41" s="26"/>
+      <c r="AL41" s="26"/>
+      <c r="AM41" s="26"/>
+      <c r="AN41" s="26"/>
+      <c r="AO41" s="26"/>
+      <c r="AP41" s="26"/>
+      <c r="AQ41" s="26"/>
+      <c r="AR41" s="26"/>
+      <c r="AS41" s="26"/>
+      <c r="AT41" s="26"/>
+      <c r="AU41" s="26"/>
+      <c r="AV41" s="26"/>
+      <c r="AW41" s="26"/>
+      <c r="AX41" s="26"/>
+      <c r="AY41" s="26"/>
+      <c r="AZ41" s="26"/>
+      <c r="BA41" s="26"/>
+      <c r="BB41" s="26"/>
+      <c r="BC41" s="26"/>
+      <c r="BD41" s="26"/>
+      <c r="BE41" s="26"/>
+      <c r="BF41" s="26"/>
+      <c r="BG41" s="26"/>
+      <c r="BH41" s="26"/>
+      <c r="BI41" s="26"/>
+      <c r="BJ41" s="26"/>
+      <c r="BK41" s="26"/>
+      <c r="BL41" s="26"/>
+      <c r="BM41" s="26"/>
+      <c r="BN41" s="26"/>
+      <c r="BO41" s="26"/>
+      <c r="BP41" s="26"/>
+      <c r="BQ41" s="26"/>
+      <c r="BR41" s="26"/>
+      <c r="BS41" s="26"/>
+      <c r="BT41" s="26"/>
+      <c r="BU41" s="26"/>
+      <c r="BV41" s="26"/>
+      <c r="BW41" s="26"/>
+      <c r="BX41" s="26"/>
+      <c r="BY41" s="26"/>
+    </row>
+    <row r="42" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="40"/>
+      <c r="B42" s="49"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="26"/>
+      <c r="I42" s="26"/>
+      <c r="J42" s="26"/>
+      <c r="K42" s="26"/>
+      <c r="L42" s="26"/>
+      <c r="M42" s="26"/>
+      <c r="N42" s="26"/>
+      <c r="O42" s="26"/>
+      <c r="P42" s="26"/>
+      <c r="Q42" s="26"/>
+      <c r="R42" s="26"/>
+      <c r="S42" s="26"/>
+      <c r="T42" s="26"/>
+      <c r="U42" s="26"/>
+      <c r="V42" s="26"/>
+      <c r="W42" s="26"/>
+      <c r="X42" s="26"/>
+      <c r="Y42" s="26"/>
+      <c r="Z42" s="26"/>
+      <c r="AA42" s="26"/>
+      <c r="AB42" s="26"/>
+      <c r="AC42" s="26"/>
+      <c r="AD42" s="26"/>
+      <c r="AE42" s="26"/>
+      <c r="AF42" s="26"/>
+      <c r="AG42" s="26"/>
+      <c r="AH42" s="26"/>
+      <c r="AI42" s="26"/>
+      <c r="AJ42" s="26"/>
+      <c r="AK42" s="26"/>
+      <c r="AL42" s="26"/>
+      <c r="AM42" s="26"/>
+      <c r="AN42" s="26"/>
+      <c r="AO42" s="26"/>
+      <c r="AP42" s="26"/>
+      <c r="AQ42" s="26"/>
+      <c r="AR42" s="26"/>
+      <c r="AS42" s="26"/>
+      <c r="AT42" s="26"/>
+      <c r="AU42" s="26"/>
+      <c r="AV42" s="26"/>
+      <c r="AW42" s="26"/>
+      <c r="AX42" s="26"/>
+      <c r="AY42" s="26"/>
+      <c r="AZ42" s="26"/>
+      <c r="BA42" s="26"/>
+      <c r="BB42" s="26"/>
+      <c r="BC42" s="26"/>
+      <c r="BD42" s="26"/>
+      <c r="BE42" s="26"/>
+      <c r="BF42" s="26"/>
+      <c r="BG42" s="26"/>
+      <c r="BH42" s="26"/>
+      <c r="BI42" s="26"/>
+      <c r="BJ42" s="26"/>
+      <c r="BK42" s="26"/>
+      <c r="BL42" s="26"/>
+      <c r="BM42" s="26"/>
+      <c r="BN42" s="26"/>
+      <c r="BO42" s="26"/>
+      <c r="BP42" s="26"/>
+      <c r="BQ42" s="26"/>
+      <c r="BR42" s="26"/>
+      <c r="BS42" s="26"/>
+      <c r="BT42" s="26"/>
+      <c r="BU42" s="26"/>
+      <c r="BV42" s="26"/>
+      <c r="BW42" s="26"/>
+      <c r="BX42" s="26"/>
+      <c r="BY42" s="26"/>
+    </row>
+    <row r="43" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="40"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="10"/>
+      <c r="G43" s="10" t="str">
         <f t="shared" si="18"/>
         <v/>
       </c>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="28"/>
-      <c r="K39" s="28"/>
-      <c r="L39" s="28"/>
-      <c r="M39" s="28"/>
-      <c r="N39" s="28"/>
-      <c r="O39" s="28"/>
-      <c r="P39" s="28"/>
-      <c r="Q39" s="28"/>
-      <c r="R39" s="28"/>
-      <c r="S39" s="28"/>
-      <c r="T39" s="28"/>
-      <c r="U39" s="28"/>
-      <c r="V39" s="28"/>
-      <c r="W39" s="28"/>
-      <c r="X39" s="28"/>
-      <c r="Y39" s="28"/>
-      <c r="Z39" s="28"/>
-      <c r="AA39" s="28"/>
-      <c r="AB39" s="28"/>
-      <c r="AC39" s="28"/>
-      <c r="AD39" s="28"/>
-      <c r="AE39" s="28"/>
-      <c r="AF39" s="28"/>
-      <c r="AG39" s="28"/>
-      <c r="AH39" s="28"/>
-      <c r="AI39" s="28"/>
-      <c r="AJ39" s="28"/>
-      <c r="AK39" s="28"/>
-      <c r="AL39" s="28"/>
-      <c r="AM39" s="28"/>
-      <c r="AN39" s="28"/>
-      <c r="AO39" s="28"/>
-      <c r="AP39" s="28"/>
-      <c r="AQ39" s="28"/>
-      <c r="AR39" s="28"/>
-      <c r="AS39" s="28"/>
-      <c r="AT39" s="28"/>
-      <c r="AU39" s="28"/>
-      <c r="AV39" s="28"/>
-      <c r="AW39" s="28"/>
-      <c r="AX39" s="28"/>
-      <c r="AY39" s="28"/>
-      <c r="AZ39" s="28"/>
-      <c r="BA39" s="28"/>
-      <c r="BB39" s="28"/>
-      <c r="BC39" s="28"/>
-      <c r="BD39" s="28"/>
-      <c r="BE39" s="28"/>
-      <c r="BF39" s="28"/>
-      <c r="BG39" s="28"/>
-      <c r="BH39" s="28"/>
-      <c r="BI39" s="28"/>
-      <c r="BJ39" s="28"/>
-      <c r="BK39" s="28"/>
-      <c r="BL39" s="28"/>
-      <c r="BM39" s="28"/>
-      <c r="BN39" s="28"/>
-      <c r="BO39" s="28"/>
-      <c r="BP39" s="28"/>
-      <c r="BQ39" s="28"/>
-      <c r="BR39" s="28"/>
-      <c r="BS39" s="28"/>
-      <c r="BT39" s="28"/>
-      <c r="BU39" s="28"/>
-      <c r="BV39" s="28"/>
-      <c r="BW39" s="28"/>
-      <c r="BX39" s="28"/>
-      <c r="BY39" s="28"/>
+      <c r="H43" s="26"/>
+      <c r="I43" s="26"/>
+      <c r="J43" s="26"/>
+      <c r="K43" s="26"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="26"/>
+      <c r="N43" s="26"/>
+      <c r="O43" s="26"/>
+      <c r="P43" s="26"/>
+      <c r="Q43" s="26"/>
+      <c r="R43" s="26"/>
+      <c r="S43" s="26"/>
+      <c r="T43" s="26"/>
+      <c r="U43" s="26"/>
+      <c r="V43" s="26"/>
+      <c r="W43" s="26"/>
+      <c r="X43" s="26"/>
+      <c r="Y43" s="26"/>
+      <c r="Z43" s="26"/>
+      <c r="AA43" s="26"/>
+      <c r="AB43" s="26"/>
+      <c r="AC43" s="26"/>
+      <c r="AD43" s="26"/>
+      <c r="AE43" s="26"/>
+      <c r="AF43" s="26"/>
+      <c r="AG43" s="26"/>
+      <c r="AH43" s="26"/>
+      <c r="AI43" s="26"/>
+      <c r="AJ43" s="26"/>
+      <c r="AK43" s="26"/>
+      <c r="AL43" s="26"/>
+      <c r="AM43" s="26"/>
+      <c r="AN43" s="26"/>
+      <c r="AO43" s="26"/>
+      <c r="AP43" s="26"/>
+      <c r="AQ43" s="26"/>
+      <c r="AR43" s="26"/>
+      <c r="AS43" s="26"/>
+      <c r="AT43" s="26"/>
+      <c r="AU43" s="26"/>
+      <c r="AV43" s="26"/>
+      <c r="AW43" s="26"/>
+      <c r="AX43" s="26"/>
+      <c r="AY43" s="26"/>
+      <c r="AZ43" s="26"/>
+      <c r="BA43" s="26"/>
+      <c r="BB43" s="26"/>
+      <c r="BC43" s="26"/>
+      <c r="BD43" s="26"/>
+      <c r="BE43" s="26"/>
+      <c r="BF43" s="26"/>
+      <c r="BG43" s="26"/>
+      <c r="BH43" s="26"/>
+      <c r="BI43" s="26"/>
+      <c r="BJ43" s="26"/>
+      <c r="BK43" s="26"/>
+      <c r="BL43" s="26"/>
+      <c r="BM43" s="26"/>
+      <c r="BN43" s="26"/>
+      <c r="BO43" s="26"/>
+      <c r="BP43" s="26"/>
+      <c r="BQ43" s="26"/>
+      <c r="BR43" s="26"/>
+      <c r="BS43" s="26"/>
+      <c r="BT43" s="26"/>
+      <c r="BU43" s="26"/>
+      <c r="BV43" s="26"/>
+      <c r="BW43" s="26"/>
+      <c r="BX43" s="26"/>
+      <c r="BY43" s="26"/>
     </row>
-    <row r="40" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F40" s="5"/>
+    <row r="44" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="50" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="9"/>
+      <c r="D44" s="67">
+        <v>45782</v>
+      </c>
+      <c r="E44" s="67">
+        <f>D44+5</f>
+        <v>45787</v>
+      </c>
+      <c r="F44" s="10"/>
+      <c r="G44" s="10">
+        <f t="shared" si="18"/>
+        <v>6</v>
+      </c>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26"/>
+      <c r="K44" s="26"/>
+      <c r="L44" s="26"/>
+      <c r="M44" s="26"/>
+      <c r="N44" s="26"/>
+      <c r="O44" s="26"/>
+      <c r="P44" s="26"/>
+      <c r="Q44" s="26"/>
+      <c r="R44" s="26"/>
+      <c r="S44" s="26"/>
+      <c r="T44" s="26"/>
+      <c r="U44" s="26"/>
+      <c r="V44" s="26"/>
+      <c r="W44" s="26"/>
+      <c r="X44" s="26"/>
+      <c r="Y44" s="26"/>
+      <c r="Z44" s="26"/>
+      <c r="AA44" s="26"/>
+      <c r="AB44" s="26"/>
+      <c r="AC44" s="26"/>
+      <c r="AD44" s="26"/>
+      <c r="AE44" s="26"/>
+      <c r="AF44" s="26"/>
+      <c r="AG44" s="26"/>
+      <c r="AH44" s="26"/>
+      <c r="AI44" s="26"/>
+      <c r="AJ44" s="26"/>
+      <c r="AK44" s="26"/>
+      <c r="AL44" s="26"/>
+      <c r="AM44" s="26"/>
+      <c r="AN44" s="26"/>
+      <c r="AO44" s="26"/>
+      <c r="AP44" s="26"/>
+      <c r="AQ44" s="26"/>
+      <c r="AR44" s="26"/>
+      <c r="AS44" s="26"/>
+      <c r="AT44" s="26"/>
+      <c r="AU44" s="26"/>
+      <c r="AV44" s="26"/>
+      <c r="AW44" s="26"/>
+      <c r="AX44" s="26"/>
+      <c r="AY44" s="26"/>
+      <c r="AZ44" s="26"/>
+      <c r="BA44" s="26"/>
+      <c r="BB44" s="26"/>
+      <c r="BC44" s="26"/>
+      <c r="BD44" s="26"/>
+      <c r="BE44" s="26"/>
+      <c r="BF44" s="26"/>
+      <c r="BG44" s="26"/>
+      <c r="BH44" s="26"/>
+      <c r="BI44" s="26"/>
+      <c r="BJ44" s="26"/>
+      <c r="BK44" s="26"/>
+      <c r="BL44" s="26"/>
+      <c r="BM44" s="26"/>
+      <c r="BN44" s="26"/>
+      <c r="BO44" s="26"/>
+      <c r="BP44" s="26"/>
+      <c r="BQ44" s="26"/>
+      <c r="BR44" s="26"/>
+      <c r="BS44" s="26"/>
+      <c r="BT44" s="26"/>
+      <c r="BU44" s="26"/>
+      <c r="BV44" s="26"/>
+      <c r="BW44" s="26"/>
+      <c r="BX44" s="26"/>
+      <c r="BY44" s="26"/>
     </row>
-    <row r="41" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E41" s="42"/>
+    <row r="45" spans="1:77" s="2" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="B45" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C45" s="24"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25" t="str">
+        <f t="shared" si="18"/>
+        <v/>
+      </c>
+      <c r="H45" s="28"/>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="28"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="T45" s="28"/>
+      <c r="U45" s="28"/>
+      <c r="V45" s="28"/>
+      <c r="W45" s="28"/>
+      <c r="X45" s="28"/>
+      <c r="Y45" s="28"/>
+      <c r="Z45" s="28"/>
+      <c r="AA45" s="28"/>
+      <c r="AB45" s="28"/>
+      <c r="AC45" s="28"/>
+      <c r="AD45" s="28"/>
+      <c r="AE45" s="28"/>
+      <c r="AF45" s="28"/>
+      <c r="AG45" s="28"/>
+      <c r="AH45" s="28"/>
+      <c r="AI45" s="28"/>
+      <c r="AJ45" s="28"/>
+      <c r="AK45" s="28"/>
+      <c r="AL45" s="28"/>
+      <c r="AM45" s="28"/>
+      <c r="AN45" s="28"/>
+      <c r="AO45" s="28"/>
+      <c r="AP45" s="28"/>
+      <c r="AQ45" s="28"/>
+      <c r="AR45" s="28"/>
+      <c r="AS45" s="28"/>
+      <c r="AT45" s="28"/>
+      <c r="AU45" s="28"/>
+      <c r="AV45" s="28"/>
+      <c r="AW45" s="28"/>
+      <c r="AX45" s="28"/>
+      <c r="AY45" s="28"/>
+      <c r="AZ45" s="28"/>
+      <c r="BA45" s="28"/>
+      <c r="BB45" s="28"/>
+      <c r="BC45" s="28"/>
+      <c r="BD45" s="28"/>
+      <c r="BE45" s="28"/>
+      <c r="BF45" s="28"/>
+      <c r="BG45" s="28"/>
+      <c r="BH45" s="28"/>
+      <c r="BI45" s="28"/>
+      <c r="BJ45" s="28"/>
+      <c r="BK45" s="28"/>
+      <c r="BL45" s="28"/>
+      <c r="BM45" s="28"/>
+      <c r="BN45" s="28"/>
+      <c r="BO45" s="28"/>
+      <c r="BP45" s="28"/>
+      <c r="BQ45" s="28"/>
+      <c r="BR45" s="28"/>
+      <c r="BS45" s="28"/>
+      <c r="BT45" s="28"/>
+      <c r="BU45" s="28"/>
+      <c r="BV45" s="28"/>
+      <c r="BW45" s="28"/>
+      <c r="BX45" s="28"/>
+      <c r="BY45" s="28"/>
+    </row>
+    <row r="46" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F46" s="5"/>
+    </row>
+    <row r="47" spans="1:77" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E47" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5636,7 +6227,7 @@
     <mergeCell ref="AQ4:AW4"/>
     <mergeCell ref="AX4:BD4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C39">
+  <conditionalFormatting sqref="C7:C45">
     <cfRule type="dataBar" priority="20">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -5650,27 +6241,27 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BJ39 BL5:BQ39 BS5:BX39">
+  <conditionalFormatting sqref="H5:BJ45 BL5:BQ45 BS5:BX45">
     <cfRule type="expression" dxfId="4" priority="39">
       <formula>AND(TODAY()&gt;=H$5,TODAY()&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BJ39 BL7:BQ39 BS7:BX39">
+  <conditionalFormatting sqref="H7:BJ45 BL7:BQ45 BS7:BX45">
     <cfRule type="expression" dxfId="3" priority="34" stopIfTrue="1">
       <formula>AND(task_end&gt;=H$5,task_start&lt;I$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:BY39">
+  <conditionalFormatting sqref="H7:BY45">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>AND(task_start&lt;=H$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=H$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK5:BK39 BR5:BR39 BY5:BY39">
+  <conditionalFormatting sqref="BK5:BK45 BR5:BR45 BY5:BY45">
     <cfRule type="expression" dxfId="1" priority="41">
       <formula>AND(TODAY()&gt;=BK$5,TODAY()&lt;BZ$5)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BK7:BK39 BR7:BR39 BY7:BY39">
+  <conditionalFormatting sqref="BK7:BK45 BR7:BR45 BY7:BY45">
     <cfRule type="expression" dxfId="0" priority="45" stopIfTrue="1">
       <formula>AND(task_end&gt;=BK$5,task_start&lt;BZ$5)</formula>
     </cfRule>
@@ -5706,7 +6297,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C39</xm:sqref>
+          <xm:sqref>C7:C45</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5729,79 +6320,79 @@
     <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:2" s="32" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" s="31"/>
     </row>
     <row r="3" spans="1:2" s="36" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="54" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B3" s="37"/>
     </row>
     <row r="4" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A4" s="34" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="74" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:2" s="30" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="39" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A8" s="34" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="64" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:2" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="38" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A11" s="34" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:2" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="38" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:2" s="33" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A14" s="34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="35" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="80" x14ac:dyDescent="0.2">
       <c r="A16" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -5818,6 +6409,35 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6105,36 +6725,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{708DBB9E-6D89-4A94-9DC5-964B7833E11C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6153,24 +6764,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8FE8ED85-58B3-4608-8E91-0433556D50CE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5144944C-1F1D-4162-962A-96F3FC8455D8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>